<commit_message>
Mudança - saída log classificação
</commit_message>
<xml_diff>
--- a/access.xlsx
+++ b/access.xlsx
@@ -137,12 +137,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -159,9 +159,9 @@
   <dimension ref="A1:D154"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E152" activeCellId="0" sqref="E152"/>
+      <selection pane="bottomLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -849,847 +849,847 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
-        <v>497</v>
+        <v>465</v>
       </c>
       <c r="B46" s="0" t="n">
-        <v>1557324393</v>
+        <v>1557327838</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D46" s="2" t="n">
         <f aca="false">(B46/86400) + 25569</f>
-        <v>43593.5878819445</v>
+        <v>43593.6277546296</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B47" s="0" t="n">
-        <v>1557327838</v>
+        <v>1557356421</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D47" s="2" t="n">
         <f aca="false">(B47/86400) + 25569</f>
-        <v>43593.6277546296</v>
+        <v>43593.9585763889</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
-        <v>498</v>
+        <v>467</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>1557327838</v>
+        <v>1557361890</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D48" s="2" t="n">
         <f aca="false">(B48/86400) + 25569</f>
-        <v>43593.6277546296</v>
+        <v>43594.021875</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>1557356421</v>
+        <v>1557401113</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D49" s="2" t="n">
         <f aca="false">(B49/86400) + 25569</f>
-        <v>43593.9585763889</v>
+        <v>43594.4758449074</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
-        <v>499</v>
+        <v>469</v>
       </c>
       <c r="B50" s="0" t="n">
-        <v>1557356421</v>
+        <v>1557401167</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D50" s="2" t="n">
         <f aca="false">(B50/86400) + 25569</f>
-        <v>43593.9585763889</v>
+        <v>43594.4764699074</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>1557361890</v>
+        <v>1557401193</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D51" s="2" t="n">
         <f aca="false">(B51/86400) + 25569</f>
-        <v>43594.021875</v>
+        <v>43594.4767708333</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
-        <v>500</v>
+        <v>471</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>1557361890</v>
+        <v>1557402687</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D52" s="2" t="n">
         <f aca="false">(B52/86400) + 25569</f>
-        <v>43594.021875</v>
+        <v>43594.4940625</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="B53" s="0" t="n">
-        <v>1557401113</v>
+        <v>1557413621</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D53" s="2" t="n">
         <f aca="false">(B53/86400) + 25569</f>
-        <v>43594.4758449074</v>
+        <v>43594.6206134259</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
-        <v>501</v>
+        <v>473</v>
       </c>
       <c r="B54" s="0" t="n">
-        <v>1557401113</v>
+        <v>1557418758</v>
       </c>
       <c r="C54" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D54" s="2" t="n">
         <f aca="false">(B54/86400) + 25569</f>
-        <v>43594.4758449074</v>
+        <v>43594.6800694444</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
-        <v>469</v>
+        <v>474</v>
       </c>
       <c r="B55" s="0" t="n">
-        <v>1557401167</v>
+        <v>1557428082</v>
       </c>
       <c r="C55" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D55" s="2" t="n">
         <f aca="false">(B55/86400) + 25569</f>
-        <v>43594.4764699074</v>
+        <v>43594.7879861111</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
-        <v>502</v>
+        <v>475</v>
       </c>
       <c r="B56" s="0" t="n">
-        <v>1557401167</v>
+        <v>1557443204</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D56" s="2" t="n">
         <f aca="false">(B56/86400) + 25569</f>
-        <v>43594.4764699074</v>
+        <v>43594.9630092593</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
-        <v>470</v>
+        <v>476</v>
       </c>
       <c r="B57" s="0" t="n">
-        <v>1557401193</v>
+        <v>1557488562</v>
       </c>
       <c r="C57" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D57" s="2" t="n">
         <f aca="false">(B57/86400) + 25569</f>
-        <v>43594.4767708333</v>
+        <v>43595.4879861111</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
-        <v>503</v>
+        <v>477</v>
       </c>
       <c r="B58" s="0" t="n">
-        <v>1557401193</v>
+        <v>1557495314</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D58" s="2" t="n">
         <f aca="false">(B58/86400) + 25569</f>
-        <v>43594.4767708333</v>
+        <v>43595.5661342593</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
-        <v>471</v>
+        <v>478</v>
       </c>
       <c r="B59" s="0" t="n">
-        <v>1557402687</v>
+        <v>1557497681</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D59" s="2" t="n">
         <f aca="false">(B59/86400) + 25569</f>
-        <v>43594.4940625</v>
+        <v>43595.5935300926</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
-        <v>504</v>
+        <v>479</v>
       </c>
       <c r="B60" s="0" t="n">
-        <v>1557402687</v>
+        <v>1557528623</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D60" s="2" t="n">
         <f aca="false">(B60/86400) + 25569</f>
-        <v>43594.4940625</v>
+        <v>43595.9516550926</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
-        <v>472</v>
+        <v>480</v>
       </c>
       <c r="B61" s="0" t="n">
-        <v>1557413621</v>
+        <v>1557530812</v>
       </c>
       <c r="C61" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D61" s="2" t="n">
         <f aca="false">(B61/86400) + 25569</f>
-        <v>43594.6206134259</v>
+        <v>43595.9769907407</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
-        <v>505</v>
+        <v>481</v>
       </c>
       <c r="B62" s="0" t="n">
-        <v>1557413621</v>
+        <v>1557589462</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D62" s="2" t="n">
         <f aca="false">(B62/86400) + 25569</f>
-        <v>43594.6206134259</v>
+        <v>43596.6558101852</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
-        <v>473</v>
+        <v>482</v>
       </c>
       <c r="B63" s="0" t="n">
-        <v>1557418758</v>
+        <v>1557589466</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D63" s="2" t="n">
         <f aca="false">(B63/86400) + 25569</f>
-        <v>43594.6800694444</v>
+        <v>43596.6558564815</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
-        <v>506</v>
+        <v>483</v>
       </c>
       <c r="B64" s="0" t="n">
-        <v>1557418758</v>
+        <v>1557589737</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D64" s="2" t="n">
         <f aca="false">(B64/86400) + 25569</f>
-        <v>43594.6800694444</v>
+        <v>43596.6589930556</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
-        <v>474</v>
+        <v>484</v>
       </c>
       <c r="B65" s="0" t="n">
-        <v>1557428082</v>
+        <v>1557589746</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D65" s="2" t="n">
         <f aca="false">(B65/86400) + 25569</f>
-        <v>43594.7879861111</v>
+        <v>43596.6590972222</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
-        <v>507</v>
+        <v>485</v>
       </c>
       <c r="B66" s="0" t="n">
-        <v>1557428082</v>
+        <v>1557589748</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D66" s="2" t="n">
         <f aca="false">(B66/86400) + 25569</f>
-        <v>43594.7879861111</v>
+        <v>43596.6591203704</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
-        <v>475</v>
+        <v>486</v>
       </c>
       <c r="B67" s="0" t="n">
-        <v>1557443204</v>
+        <v>1557589751</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D67" s="2" t="n">
         <f aca="false">(B67/86400) + 25569</f>
-        <v>43594.9630092593</v>
+        <v>43596.6591550926</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
-        <v>508</v>
+        <v>487</v>
       </c>
       <c r="B68" s="0" t="n">
-        <v>1557443204</v>
+        <v>1557589762</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D68" s="2" t="n">
         <f aca="false">(B68/86400) + 25569</f>
-        <v>43594.9630092593</v>
+        <v>43596.6592824074</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
-        <v>476</v>
+        <v>488</v>
       </c>
       <c r="B69" s="0" t="n">
-        <v>1557488562</v>
+        <v>1557589764</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D69" s="2" t="n">
         <f aca="false">(B69/86400) + 25569</f>
-        <v>43595.4879861111</v>
+        <v>43596.6593055556</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
-        <v>509</v>
+        <v>489</v>
       </c>
       <c r="B70" s="0" t="n">
-        <v>1557488562</v>
+        <v>1557589768</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D70" s="2" t="n">
         <f aca="false">(B70/86400) + 25569</f>
-        <v>43595.4879861111</v>
+        <v>43596.6593518519</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
-        <v>477</v>
+        <v>490</v>
       </c>
       <c r="B71" s="0" t="n">
-        <v>1557495314</v>
+        <v>1557589771</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D71" s="2" t="n">
         <f aca="false">(B71/86400) + 25569</f>
-        <v>43595.5661342593</v>
+        <v>43596.6593865741</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
-        <v>510</v>
+        <v>491</v>
       </c>
       <c r="B72" s="0" t="n">
-        <v>1557495314</v>
+        <v>1557589777</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D72" s="2" t="n">
         <f aca="false">(B72/86400) + 25569</f>
-        <v>43595.5661342593</v>
+        <v>43596.6594560185</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
-        <v>478</v>
+        <v>492</v>
       </c>
       <c r="B73" s="0" t="n">
-        <v>1557497681</v>
+        <v>1557589780</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D73" s="2" t="n">
         <f aca="false">(B73/86400) + 25569</f>
-        <v>43595.5935300926</v>
+        <v>43596.6594907407</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
-        <v>511</v>
+        <v>493</v>
       </c>
       <c r="B74" s="0" t="n">
-        <v>1557497681</v>
+        <v>1557589791</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D74" s="2" t="n">
         <f aca="false">(B74/86400) + 25569</f>
-        <v>43595.5935300926</v>
+        <v>43596.6596180556</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
-        <v>479</v>
+        <v>494</v>
       </c>
       <c r="B75" s="0" t="n">
-        <v>1557528623</v>
+        <v>1557589805</v>
       </c>
       <c r="C75" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D75" s="2" t="n">
         <f aca="false">(B75/86400) + 25569</f>
-        <v>43595.9516550926</v>
+        <v>43596.6597800926</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
-        <v>512</v>
+        <v>495</v>
       </c>
       <c r="B76" s="0" t="n">
-        <v>1557528623</v>
+        <v>1557589809</v>
       </c>
       <c r="C76" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D76" s="2" t="n">
         <f aca="false">(B76/86400) + 25569</f>
-        <v>43595.9516550926</v>
+        <v>43596.6598263889</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
-        <v>480</v>
+        <v>496</v>
       </c>
       <c r="B77" s="0" t="n">
-        <v>1557530812</v>
+        <v>1557590119</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D77" s="2" t="n">
         <f aca="false">(B77/86400) + 25569</f>
-        <v>43595.9769907407</v>
+        <v>43596.6634143519</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
-        <v>513</v>
+        <v>497</v>
       </c>
       <c r="B78" s="0" t="n">
-        <v>1557530812</v>
+        <v>1557324393</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D78" s="2" t="n">
         <f aca="false">(B78/86400) + 25569</f>
-        <v>43595.9769907407</v>
+        <v>43593.5878819445</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="n">
-        <v>481</v>
+        <v>498</v>
       </c>
       <c r="B79" s="0" t="n">
-        <v>1557589462</v>
+        <v>1557327838</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D79" s="2" t="n">
         <f aca="false">(B79/86400) + 25569</f>
-        <v>43596.6558101852</v>
+        <v>43593.6277546296</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
-        <v>514</v>
+        <v>499</v>
       </c>
       <c r="B80" s="0" t="n">
-        <v>1557589462</v>
+        <v>1557356421</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D80" s="2" t="n">
         <f aca="false">(B80/86400) + 25569</f>
-        <v>43596.6558101852</v>
+        <v>43593.9585763889</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="n">
-        <v>544</v>
+        <v>500</v>
       </c>
       <c r="B81" s="0" t="n">
-        <v>1557589462</v>
+        <v>1557361890</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D81" s="2" t="n">
         <f aca="false">(B81/86400) + 25569</f>
-        <v>43596.6558101852</v>
+        <v>43594.021875</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
-        <v>482</v>
+        <v>501</v>
       </c>
       <c r="B82" s="0" t="n">
-        <v>1557589466</v>
+        <v>1557401113</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D82" s="2" t="n">
         <f aca="false">(B82/86400) + 25569</f>
-        <v>43596.6558564815</v>
+        <v>43594.4758449074</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="n">
-        <v>515</v>
+        <v>502</v>
       </c>
       <c r="B83" s="0" t="n">
-        <v>1557589466</v>
+        <v>1557401167</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D83" s="2" t="n">
         <f aca="false">(B83/86400) + 25569</f>
-        <v>43596.6558564815</v>
+        <v>43594.4764699074</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
-        <v>545</v>
+        <v>503</v>
       </c>
       <c r="B84" s="0" t="n">
-        <v>1557589466</v>
+        <v>1557401193</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D84" s="2" t="n">
         <f aca="false">(B84/86400) + 25569</f>
-        <v>43596.6558564815</v>
+        <v>43594.4767708333</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="n">
-        <v>483</v>
+        <v>504</v>
       </c>
       <c r="B85" s="0" t="n">
-        <v>1557589737</v>
+        <v>1557402687</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D85" s="2" t="n">
         <f aca="false">(B85/86400) + 25569</f>
-        <v>43596.6589930556</v>
+        <v>43594.4940625</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="n">
-        <v>516</v>
+        <v>505</v>
       </c>
       <c r="B86" s="0" t="n">
-        <v>1557589737</v>
+        <v>1557413621</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D86" s="2" t="n">
         <f aca="false">(B86/86400) + 25569</f>
-        <v>43596.6589930556</v>
+        <v>43594.6206134259</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="n">
-        <v>546</v>
+        <v>506</v>
       </c>
       <c r="B87" s="0" t="n">
-        <v>1557589737</v>
+        <v>1557418758</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D87" s="2" t="n">
         <f aca="false">(B87/86400) + 25569</f>
-        <v>43596.6589930556</v>
+        <v>43594.6800694444</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="n">
-        <v>484</v>
+        <v>507</v>
       </c>
       <c r="B88" s="0" t="n">
-        <v>1557589746</v>
+        <v>1557428082</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D88" s="2" t="n">
         <f aca="false">(B88/86400) + 25569</f>
-        <v>43596.6590972222</v>
+        <v>43594.7879861111</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="n">
-        <v>517</v>
+        <v>508</v>
       </c>
       <c r="B89" s="0" t="n">
-        <v>1557589746</v>
+        <v>1557443204</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D89" s="2" t="n">
         <f aca="false">(B89/86400) + 25569</f>
-        <v>43596.6590972222</v>
+        <v>43594.9630092593</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="n">
-        <v>547</v>
+        <v>509</v>
       </c>
       <c r="B90" s="0" t="n">
-        <v>1557589746</v>
+        <v>1557488562</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D90" s="2" t="n">
         <f aca="false">(B90/86400) + 25569</f>
-        <v>43596.6590972222</v>
+        <v>43595.4879861111</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="n">
-        <v>485</v>
+        <v>510</v>
       </c>
       <c r="B91" s="0" t="n">
-        <v>1557589748</v>
+        <v>1557495314</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D91" s="2" t="n">
         <f aca="false">(B91/86400) + 25569</f>
-        <v>43596.6591203704</v>
+        <v>43595.5661342593</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="n">
-        <v>518</v>
+        <v>511</v>
       </c>
       <c r="B92" s="0" t="n">
-        <v>1557589748</v>
+        <v>1557497681</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D92" s="2" t="n">
         <f aca="false">(B92/86400) + 25569</f>
-        <v>43596.6591203704</v>
+        <v>43595.5935300926</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="n">
-        <v>548</v>
+        <v>512</v>
       </c>
       <c r="B93" s="0" t="n">
-        <v>1557589748</v>
+        <v>1557528623</v>
       </c>
       <c r="C93" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D93" s="2" t="n">
         <f aca="false">(B93/86400) + 25569</f>
-        <v>43596.6591203704</v>
+        <v>43595.9516550926</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="n">
-        <v>486</v>
+        <v>513</v>
       </c>
       <c r="B94" s="0" t="n">
-        <v>1557589751</v>
+        <v>1557530812</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D94" s="2" t="n">
         <f aca="false">(B94/86400) + 25569</f>
-        <v>43596.6591550926</v>
+        <v>43595.9769907407</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="n">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="B95" s="0" t="n">
-        <v>1557589751</v>
+        <v>1557589462</v>
       </c>
       <c r="C95" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D95" s="2" t="n">
         <f aca="false">(B95/86400) + 25569</f>
-        <v>43596.6591550926</v>
+        <v>43596.6558101852</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="n">
-        <v>549</v>
+        <v>515</v>
       </c>
       <c r="B96" s="0" t="n">
-        <v>1557589751</v>
+        <v>1557589466</v>
       </c>
       <c r="C96" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D96" s="2" t="n">
         <f aca="false">(B96/86400) + 25569</f>
-        <v>43596.6591550926</v>
+        <v>43596.6558564815</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="n">
-        <v>487</v>
+        <v>516</v>
       </c>
       <c r="B97" s="0" t="n">
-        <v>1557589762</v>
+        <v>1557589737</v>
       </c>
       <c r="C97" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D97" s="2" t="n">
         <f aca="false">(B97/86400) + 25569</f>
-        <v>43596.6592824074</v>
+        <v>43596.6589930556</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="n">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="B98" s="0" t="n">
-        <v>1557589762</v>
+        <v>1557589746</v>
       </c>
       <c r="C98" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D98" s="2" t="n">
         <f aca="false">(B98/86400) + 25569</f>
-        <v>43596.6592824074</v>
+        <v>43596.6590972222</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="n">
-        <v>550</v>
+        <v>518</v>
       </c>
       <c r="B99" s="0" t="n">
-        <v>1557589762</v>
+        <v>1557589748</v>
       </c>
       <c r="C99" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D99" s="2" t="n">
         <f aca="false">(B99/86400) + 25569</f>
-        <v>43596.6592824074</v>
+        <v>43596.6591203704</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="n">
-        <v>488</v>
+        <v>519</v>
       </c>
       <c r="B100" s="0" t="n">
-        <v>1557589764</v>
+        <v>1557589751</v>
       </c>
       <c r="C100" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D100" s="2" t="n">
         <f aca="false">(B100/86400) + 25569</f>
-        <v>43596.6593055556</v>
+        <v>43596.6591550926</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="n">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B101" s="0" t="n">
-        <v>1557589764</v>
+        <v>1557589762</v>
       </c>
       <c r="C101" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D101" s="2" t="n">
         <f aca="false">(B101/86400) + 25569</f>
-        <v>43596.6593055556</v>
+        <v>43596.6592824074</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="n">
-        <v>551</v>
+        <v>521</v>
       </c>
       <c r="B102" s="0" t="n">
         <v>1557589764</v>
@@ -1704,7 +1704,7 @@
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="n">
-        <v>489</v>
+        <v>522</v>
       </c>
       <c r="B103" s="0" t="n">
         <v>1557589768</v>
@@ -1719,752 +1719,752 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="n">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B104" s="0" t="n">
-        <v>1557589768</v>
+        <v>1557589771</v>
       </c>
       <c r="C104" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D104" s="2" t="n">
         <f aca="false">(B104/86400) + 25569</f>
-        <v>43596.6593518519</v>
+        <v>43596.6593865741</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="n">
-        <v>552</v>
+        <v>524</v>
       </c>
       <c r="B105" s="0" t="n">
-        <v>1557589768</v>
+        <v>1557589777</v>
       </c>
       <c r="C105" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D105" s="2" t="n">
         <f aca="false">(B105/86400) + 25569</f>
-        <v>43596.6593518519</v>
+        <v>43596.6594560185</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="n">
-        <v>490</v>
+        <v>525</v>
       </c>
       <c r="B106" s="0" t="n">
-        <v>1557589771</v>
+        <v>1557589780</v>
       </c>
       <c r="C106" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D106" s="2" t="n">
         <f aca="false">(B106/86400) + 25569</f>
-        <v>43596.6593865741</v>
+        <v>43596.6594907407</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="n">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="B107" s="0" t="n">
-        <v>1557589771</v>
+        <v>1557589791</v>
       </c>
       <c r="C107" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D107" s="2" t="n">
         <f aca="false">(B107/86400) + 25569</f>
-        <v>43596.6593865741</v>
+        <v>43596.6596180556</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="n">
-        <v>553</v>
+        <v>527</v>
       </c>
       <c r="B108" s="0" t="n">
-        <v>1557589771</v>
+        <v>1557589805</v>
       </c>
       <c r="C108" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D108" s="2" t="n">
         <f aca="false">(B108/86400) + 25569</f>
-        <v>43596.6593865741</v>
+        <v>43596.6597800926</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="n">
-        <v>491</v>
+        <v>528</v>
       </c>
       <c r="B109" s="0" t="n">
-        <v>1557589777</v>
+        <v>1557589809</v>
       </c>
       <c r="C109" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D109" s="2" t="n">
         <f aca="false">(B109/86400) + 25569</f>
-        <v>43596.6594560185</v>
+        <v>43596.6598263889</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="n">
-        <v>524</v>
+        <v>529</v>
       </c>
       <c r="B110" s="0" t="n">
-        <v>1557589777</v>
+        <v>1557590119</v>
       </c>
       <c r="C110" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D110" s="2" t="n">
         <f aca="false">(B110/86400) + 25569</f>
-        <v>43596.6594560185</v>
+        <v>43596.6634143519</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="n">
-        <v>554</v>
+        <v>530</v>
       </c>
       <c r="B111" s="0" t="n">
-        <v>1557589777</v>
+        <v>1557736101</v>
       </c>
       <c r="C111" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D111" s="2" t="n">
         <f aca="false">(B111/86400) + 25569</f>
-        <v>43596.6594560185</v>
+        <v>43598.3530208333</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="n">
-        <v>492</v>
+        <v>531</v>
       </c>
       <c r="B112" s="0" t="n">
-        <v>1557589780</v>
+        <v>1557758822</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D112" s="2" t="n">
         <f aca="false">(B112/86400) + 25569</f>
-        <v>43596.6594907407</v>
+        <v>43598.6159953704</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="n">
-        <v>525</v>
+        <v>532</v>
       </c>
       <c r="B113" s="0" t="n">
-        <v>1557589780</v>
+        <v>1557786190</v>
       </c>
       <c r="C113" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D113" s="2" t="n">
         <f aca="false">(B113/86400) + 25569</f>
-        <v>43596.6594907407</v>
+        <v>43598.9327546296</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="n">
-        <v>555</v>
+        <v>533</v>
       </c>
       <c r="B114" s="0" t="n">
-        <v>1557589780</v>
+        <v>1557786411</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D114" s="2" t="n">
         <f aca="false">(B114/86400) + 25569</f>
-        <v>43596.6594907407</v>
+        <v>43598.9353125</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="n">
-        <v>493</v>
+        <v>534</v>
       </c>
       <c r="B115" s="0" t="n">
-        <v>1557589791</v>
+        <v>1557789585</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D115" s="2" t="n">
         <f aca="false">(B115/86400) + 25569</f>
-        <v>43596.6596180556</v>
+        <v>43598.9720486111</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="n">
-        <v>526</v>
+        <v>535</v>
       </c>
       <c r="B116" s="0" t="n">
-        <v>1557589791</v>
+        <v>1557789692</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D116" s="2" t="n">
         <f aca="false">(B116/86400) + 25569</f>
-        <v>43596.6596180556</v>
+        <v>43598.973287037</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="n">
-        <v>556</v>
+        <v>536</v>
       </c>
       <c r="B117" s="0" t="n">
-        <v>1557589791</v>
+        <v>1557789797</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D117" s="2" t="n">
         <f aca="false">(B117/86400) + 25569</f>
-        <v>43596.6596180556</v>
+        <v>43598.9745023148</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="n">
-        <v>494</v>
+        <v>537</v>
       </c>
       <c r="B118" s="0" t="n">
-        <v>1557589805</v>
+        <v>1557791622</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D118" s="2" t="n">
         <f aca="false">(B118/86400) + 25569</f>
-        <v>43596.6597800926</v>
+        <v>43598.995625</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="n">
-        <v>527</v>
+        <v>538</v>
       </c>
       <c r="B119" s="0" t="n">
-        <v>1557589805</v>
+        <v>1557795012</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D119" s="2" t="n">
         <f aca="false">(B119/86400) + 25569</f>
-        <v>43596.6597800926</v>
+        <v>43599.0348611111</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="n">
-        <v>557</v>
+        <v>539</v>
       </c>
       <c r="B120" s="0" t="n">
-        <v>1557589805</v>
+        <v>1557828829</v>
       </c>
       <c r="C120" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D120" s="2" t="n">
         <f aca="false">(B120/86400) + 25569</f>
-        <v>43596.6597800926</v>
+        <v>43599.4262615741</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="n">
-        <v>495</v>
+        <v>540</v>
       </c>
       <c r="B121" s="0" t="n">
-        <v>1557589809</v>
+        <v>1557839756</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D121" s="2" t="n">
         <f aca="false">(B121/86400) + 25569</f>
-        <v>43596.6598263889</v>
+        <v>43599.5527314815</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="n">
-        <v>528</v>
+        <v>541</v>
       </c>
       <c r="B122" s="0" t="n">
-        <v>1557589809</v>
+        <v>1557842855</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D122" s="2" t="n">
         <f aca="false">(B122/86400) + 25569</f>
-        <v>43596.6598263889</v>
+        <v>43599.588599537</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="n">
-        <v>558</v>
+        <v>542</v>
       </c>
       <c r="B123" s="0" t="n">
-        <v>1557589809</v>
+        <v>1557848174</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D123" s="2" t="n">
         <f aca="false">(B123/86400) + 25569</f>
-        <v>43596.6598263889</v>
+        <v>43599.650162037</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="n">
-        <v>496</v>
+        <v>543</v>
       </c>
       <c r="B124" s="0" t="n">
-        <v>1557590119</v>
+        <v>1557880519</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D124" s="2" t="n">
         <f aca="false">(B124/86400) + 25569</f>
-        <v>43596.6634143519</v>
+        <v>43600.024525463</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="n">
-        <v>529</v>
+        <v>544</v>
       </c>
       <c r="B125" s="0" t="n">
-        <v>1557590119</v>
+        <v>1557589462</v>
       </c>
       <c r="C125" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D125" s="2" t="n">
         <f aca="false">(B125/86400) + 25569</f>
-        <v>43596.6634143519</v>
+        <v>43596.6558101852</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="n">
-        <v>559</v>
+        <v>545</v>
       </c>
       <c r="B126" s="0" t="n">
-        <v>1557590119</v>
+        <v>1557589466</v>
       </c>
       <c r="C126" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D126" s="2" t="n">
         <f aca="false">(B126/86400) + 25569</f>
-        <v>43596.6634143519</v>
+        <v>43596.6558564815</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="n">
-        <v>530</v>
+        <v>546</v>
       </c>
       <c r="B127" s="0" t="n">
-        <v>1557736101</v>
+        <v>1557589737</v>
       </c>
       <c r="C127" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D127" s="2" t="n">
         <f aca="false">(B127/86400) + 25569</f>
-        <v>43598.3530208333</v>
+        <v>43596.6589930556</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="n">
-        <v>560</v>
+        <v>547</v>
       </c>
       <c r="B128" s="0" t="n">
-        <v>1557736101</v>
+        <v>1557589746</v>
       </c>
       <c r="C128" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D128" s="2" t="n">
         <f aca="false">(B128/86400) + 25569</f>
-        <v>43598.3530208333</v>
+        <v>43596.6590972222</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="n">
-        <v>531</v>
+        <v>548</v>
       </c>
       <c r="B129" s="0" t="n">
-        <v>1557758822</v>
+        <v>1557589748</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D129" s="2" t="n">
         <f aca="false">(B129/86400) + 25569</f>
-        <v>43598.6159953704</v>
+        <v>43596.6591203704</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="n">
-        <v>561</v>
+        <v>549</v>
       </c>
       <c r="B130" s="0" t="n">
-        <v>1557758822</v>
+        <v>1557589751</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D130" s="2" t="n">
         <f aca="false">(B130/86400) + 25569</f>
-        <v>43598.6159953704</v>
+        <v>43596.6591550926</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="n">
-        <v>532</v>
+        <v>550</v>
       </c>
       <c r="B131" s="0" t="n">
-        <v>1557786190</v>
+        <v>1557589762</v>
       </c>
       <c r="C131" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D131" s="2" t="n">
         <f aca="false">(B131/86400) + 25569</f>
-        <v>43598.9327546296</v>
+        <v>43596.6592824074</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="n">
-        <v>562</v>
+        <v>551</v>
       </c>
       <c r="B132" s="0" t="n">
-        <v>1557786190</v>
+        <v>1557589764</v>
       </c>
       <c r="C132" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D132" s="2" t="n">
         <f aca="false">(B132/86400) + 25569</f>
-        <v>43598.9327546296</v>
+        <v>43596.6593055556</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="n">
-        <v>533</v>
+        <v>552</v>
       </c>
       <c r="B133" s="0" t="n">
-        <v>1557786411</v>
+        <v>1557589768</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D133" s="2" t="n">
         <f aca="false">(B133/86400) + 25569</f>
-        <v>43598.9353125</v>
+        <v>43596.6593518519</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="n">
-        <v>563</v>
+        <v>553</v>
       </c>
       <c r="B134" s="0" t="n">
-        <v>1557786411</v>
+        <v>1557589771</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D134" s="2" t="n">
         <f aca="false">(B134/86400) + 25569</f>
-        <v>43598.9353125</v>
+        <v>43596.6593865741</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="n">
-        <v>534</v>
+        <v>554</v>
       </c>
       <c r="B135" s="0" t="n">
-        <v>1557789585</v>
+        <v>1557589777</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D135" s="2" t="n">
         <f aca="false">(B135/86400) + 25569</f>
-        <v>43598.9720486111</v>
+        <v>43596.6594560185</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="n">
-        <v>564</v>
+        <v>555</v>
       </c>
       <c r="B136" s="0" t="n">
-        <v>1557789585</v>
+        <v>1557589780</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D136" s="2" t="n">
         <f aca="false">(B136/86400) + 25569</f>
-        <v>43598.9720486111</v>
+        <v>43596.6594907407</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="n">
-        <v>535</v>
+        <v>556</v>
       </c>
       <c r="B137" s="0" t="n">
-        <v>1557789692</v>
+        <v>1557589791</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D137" s="2" t="n">
         <f aca="false">(B137/86400) + 25569</f>
-        <v>43598.973287037</v>
+        <v>43596.6596180556</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="n">
-        <v>565</v>
+        <v>557</v>
       </c>
       <c r="B138" s="0" t="n">
-        <v>1557789692</v>
+        <v>1557589805</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D138" s="2" t="n">
         <f aca="false">(B138/86400) + 25569</f>
-        <v>43598.973287037</v>
+        <v>43596.6597800926</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="n">
-        <v>536</v>
+        <v>558</v>
       </c>
       <c r="B139" s="0" t="n">
-        <v>1557789797</v>
+        <v>1557589809</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D139" s="2" t="n">
         <f aca="false">(B139/86400) + 25569</f>
-        <v>43598.9745023148</v>
+        <v>43596.6598263889</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="n">
-        <v>566</v>
+        <v>559</v>
       </c>
       <c r="B140" s="0" t="n">
-        <v>1557789797</v>
+        <v>1557590119</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D140" s="2" t="n">
         <f aca="false">(B140/86400) + 25569</f>
-        <v>43598.9745023148</v>
+        <v>43596.6634143519</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="n">
-        <v>537</v>
+        <v>560</v>
       </c>
       <c r="B141" s="0" t="n">
-        <v>1557791622</v>
+        <v>1557736101</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D141" s="2" t="n">
         <f aca="false">(B141/86400) + 25569</f>
-        <v>43598.995625</v>
+        <v>43598.3530208333</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="n">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="B142" s="0" t="n">
-        <v>1557791622</v>
+        <v>1557758822</v>
       </c>
       <c r="C142" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D142" s="2" t="n">
         <f aca="false">(B142/86400) + 25569</f>
-        <v>43598.995625</v>
+        <v>43598.6159953704</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="n">
-        <v>538</v>
+        <v>562</v>
       </c>
       <c r="B143" s="0" t="n">
-        <v>1557795012</v>
+        <v>1557786190</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D143" s="2" t="n">
         <f aca="false">(B143/86400) + 25569</f>
-        <v>43599.0348611111</v>
+        <v>43598.9327546296</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="n">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="B144" s="0" t="n">
-        <v>1557795012</v>
+        <v>1557786411</v>
       </c>
       <c r="C144" s="0" t="s">
         <v>4</v>
       </c>
       <c r="D144" s="2" t="n">
         <f aca="false">(B144/86400) + 25569</f>
-        <v>43599.0348611111</v>
+        <v>43598.9353125</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="n">
-        <v>539</v>
+        <v>564</v>
       </c>
       <c r="B145" s="0" t="n">
-        <v>1557828829</v>
+        <v>1557789585</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D145" s="2" t="n">
         <f aca="false">(B145/86400) + 25569</f>
-        <v>43599.4262615741</v>
+        <v>43598.9720486111</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="n">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="B146" s="0" t="n">
-        <v>1557828829</v>
+        <v>1557789692</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D146" s="2" t="n">
         <f aca="false">(B146/86400) + 25569</f>
-        <v>43599.4262615741</v>
+        <v>43598.973287037</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="n">
-        <v>540</v>
+        <v>566</v>
       </c>
       <c r="B147" s="0" t="n">
-        <v>1557839756</v>
+        <v>1557789797</v>
       </c>
       <c r="C147" s="0" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D147" s="2" t="n">
         <f aca="false">(B147/86400) + 25569</f>
-        <v>43599.5527314815</v>
+        <v>43598.9745023148</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="n">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="B148" s="0" t="n">
-        <v>1557839756</v>
+        <v>1557791622</v>
       </c>
       <c r="C148" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D148" s="2" t="n">
         <f aca="false">(B148/86400) + 25569</f>
-        <v>43599.5527314815</v>
+        <v>43598.995625</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="n">
-        <v>541</v>
+        <v>568</v>
       </c>
       <c r="B149" s="0" t="n">
-        <v>1557842855</v>
+        <v>1557795012</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D149" s="2" t="n">
         <f aca="false">(B149/86400) + 25569</f>
-        <v>43599.588599537</v>
+        <v>43599.0348611111</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="n">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B150" s="0" t="n">
-        <v>1557842855</v>
+        <v>1557828829</v>
       </c>
       <c r="C150" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D150" s="2" t="n">
         <f aca="false">(B150/86400) + 25569</f>
-        <v>43599.588599537</v>
+        <v>43599.4262615741</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="n">
-        <v>542</v>
+        <v>570</v>
       </c>
       <c r="B151" s="0" t="n">
-        <v>1557848174</v>
+        <v>1557839756</v>
       </c>
       <c r="C151" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D151" s="2" t="n">
         <f aca="false">(B151/86400) + 25569</f>
-        <v>43599.650162037</v>
+        <v>43599.5527314815</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="n">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B152" s="0" t="n">
-        <v>1557848174</v>
+        <v>1557842855</v>
       </c>
       <c r="C152" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D152" s="2" t="n">
         <f aca="false">(B152/86400) + 25569</f>
-        <v>43599.650162037</v>
+        <v>43599.588599537</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="n">
-        <v>543</v>
+        <v>572</v>
       </c>
       <c r="B153" s="0" t="n">
-        <v>1557880519</v>
+        <v>1557848174</v>
       </c>
       <c r="C153" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D153" s="2" t="n">
         <f aca="false">(B153/86400) + 25569</f>
-        <v>43600.024525463</v>
+        <v>43599.650162037</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>